<commit_message>
modified xlsx file in static
</commit_message>
<xml_diff>
--- a/static/myexcel.xlsx
+++ b/static/myexcel.xlsx
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>jj</t>
   </si>
   <si>
     <t>hhh</t>
+  </si>
+  <si>
+    <t>hh</t>
   </si>
 </sst>
 </file>
@@ -353,32 +356,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:14">
       <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:14">
       <c r="F5" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="N7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="J9" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>